<commit_message>
most basic metadata provider for Excel
</commit_message>
<xml_diff>
--- a/src/Samples/SampleData.xlsx
+++ b/src/Samples/SampleData.xlsx
@@ -8,14 +8,13 @@
   </bookViews>
   <sheets>
     <sheet name="SalesOrders" sheetId="1" r:id="rId1"/>
-    <sheet name="MyLinks" sheetId="5" r:id="rId2"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="26">
   <si>
     <t>Region</t>
   </si>
@@ -86,39 +85,6 @@
     <t>OrderDate</t>
   </si>
   <si>
-    <t>Chandoo's Project Management Templates</t>
-  </si>
-  <si>
-    <t>ExcelUser Dashboards</t>
-  </si>
-  <si>
-    <t>Jon Peltier's Excel Chart Utilities</t>
-  </si>
-  <si>
-    <t>Contextures Recommends</t>
-  </si>
-  <si>
-    <t>Excel Pivot Tables Blog</t>
-  </si>
-  <si>
-    <t>Contextures Excel Blog</t>
-  </si>
-  <si>
-    <t>Contextures Excel Tips Website</t>
-  </si>
-  <si>
-    <t>Contextures Links</t>
-  </si>
-  <si>
-    <t>Debra's Pivot Table Books on Amazon</t>
-  </si>
-  <si>
-    <t>30 Excel Functions in 30 Days eBook Kit</t>
-  </si>
-  <si>
-    <t>JP's Random Data Generator for Excel</t>
-  </si>
-  <si>
     <t>Central</t>
   </si>
   <si>
@@ -126,12 +92,6 @@
   </si>
   <si>
     <t>East</t>
-  </si>
-  <si>
-    <t>Chandoo's Excel VBA School</t>
-  </si>
-  <si>
-    <t>Excel Guru Magic of Pivot Tables Course</t>
   </si>
 </sst>
 </file>
@@ -139,10 +99,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
-    <numFmt numFmtId="171" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="180" formatCode="m/d/yy;@"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="m/d/yy;@"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <name val="Arial Narrow"/>
@@ -174,19 +134,6 @@
       <family val="2"/>
     </font>
     <font>
-      <u/>
-      <sz val="12"/>
-      <color indexed="12"/>
-      <name val="Arial Narrow"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="14"/>
-      <name val="Arial Narrow"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="12"/>
       <name val="Arial Narrow"/>
       <family val="2"/>
@@ -209,20 +156,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="8">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="171" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="top"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
@@ -230,7 +173,7 @@
     <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -246,45 +189,39 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="180" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="171" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="171" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="5"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="4" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="8">
+  <cellStyles count="7">
     <cellStyle name="Comma 2" xfId="2"/>
     <cellStyle name="Currency_TapePivot" xfId="3"/>
     <cellStyle name="Dziesiętny" xfId="1" builtinId="3"/>
-    <cellStyle name="Hiperłącze" xfId="4" builtinId="8"/>
-    <cellStyle name="Normal 2" xfId="5"/>
-    <cellStyle name="Normal_Sheet1" xfId="6"/>
-    <cellStyle name="Normal_TapePivot" xfId="7"/>
+    <cellStyle name="Normal 2" xfId="4"/>
+    <cellStyle name="Normal_Sheet1" xfId="5"/>
+    <cellStyle name="Normal_TapePivot" xfId="6"/>
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -631,7 +568,7 @@
         <v>40184</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="C2" s="10" t="s">
         <v>7</v>
@@ -655,7 +592,7 @@
         <v>40201</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="C3" s="9" t="s">
         <v>8</v>
@@ -679,7 +616,7 @@
         <v>40218</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="C4" s="10" t="s">
         <v>6</v>
@@ -703,7 +640,7 @@
         <v>40235</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="C5" s="10" t="s">
         <v>5</v>
@@ -727,7 +664,7 @@
         <v>40252</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="C6" s="10" t="s">
         <v>13</v>
@@ -751,7 +688,7 @@
         <v>40269</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="C7" s="9" t="s">
         <v>7</v>
@@ -775,7 +712,7 @@
         <v>40286</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="C8" s="10" t="s">
         <v>18</v>
@@ -799,7 +736,7 @@
         <v>40303</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="C9" s="10" t="s">
         <v>6</v>
@@ -823,7 +760,7 @@
         <v>40320</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="C10" s="9" t="s">
         <v>9</v>
@@ -847,7 +784,7 @@
         <v>40337</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="C11" s="9" t="s">
         <v>7</v>
@@ -871,7 +808,7 @@
         <v>40354</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="C12" s="9" t="s">
         <v>12</v>
@@ -895,7 +832,7 @@
         <v>40371</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="C13" s="9" t="s">
         <v>11</v>
@@ -919,7 +856,7 @@
         <v>40388</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="C14" s="10" t="s">
         <v>19</v>
@@ -943,7 +880,7 @@
         <v>40405</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="C15" s="10" t="s">
         <v>7</v>
@@ -967,7 +904,7 @@
         <v>40422</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="C16" s="10" t="s">
         <v>10</v>
@@ -991,7 +928,7 @@
         <v>40439</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="C17" s="9" t="s">
         <v>7</v>
@@ -1015,7 +952,7 @@
         <v>40456</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="C18" s="9" t="s">
         <v>12</v>
@@ -1039,7 +976,7 @@
         <v>40473</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="C19" s="9" t="s">
         <v>7</v>
@@ -1063,7 +1000,7 @@
         <v>40490</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="C20" s="10" t="s">
         <v>19</v>
@@ -1087,7 +1024,7 @@
         <v>40507</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="C21" s="10" t="s">
         <v>8</v>
@@ -1111,7 +1048,7 @@
         <v>40524</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="C22" s="10" t="s">
         <v>10</v>
@@ -1135,7 +1072,7 @@
         <v>40541</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="C23" s="10" t="s">
         <v>19</v>
@@ -1159,7 +1096,7 @@
         <v>40558</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="C24" s="10" t="s">
         <v>5</v>
@@ -1183,7 +1120,7 @@
         <v>40575</v>
       </c>
       <c r="B25" s="10" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="C25" s="10" t="s">
         <v>10</v>
@@ -1207,7 +1144,7 @@
         <v>40592</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="C26" s="9" t="s">
         <v>7</v>
@@ -1231,7 +1168,7 @@
         <v>40609</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="C27" s="10" t="s">
         <v>13</v>
@@ -1255,7 +1192,7 @@
         <v>40626</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="C28" s="10" t="s">
         <v>6</v>
@@ -1279,7 +1216,7 @@
         <v>40643</v>
       </c>
       <c r="B29" s="10" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="C29" s="10" t="s">
         <v>18</v>
@@ -1303,7 +1240,7 @@
         <v>40660</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="C30" s="9" t="s">
         <v>11</v>
@@ -1327,7 +1264,7 @@
         <v>40677</v>
       </c>
       <c r="B31" s="10" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="C31" s="10" t="s">
         <v>5</v>
@@ -1351,7 +1288,7 @@
         <v>40694</v>
       </c>
       <c r="B32" s="10" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="C32" s="10" t="s">
         <v>5</v>
@@ -1375,7 +1312,7 @@
         <v>40711</v>
       </c>
       <c r="B33" s="9" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="C33" s="9" t="s">
         <v>8</v>
@@ -1399,7 +1336,7 @@
         <v>40728</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="C34" s="10" t="s">
         <v>7</v>
@@ -1423,7 +1360,7 @@
         <v>40745</v>
       </c>
       <c r="B35" s="9" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="C35" s="9" t="s">
         <v>12</v>
@@ -1447,7 +1384,7 @@
         <v>40762</v>
       </c>
       <c r="B36" s="9" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="C36" s="10" t="s">
         <v>8</v>
@@ -1471,7 +1408,7 @@
         <v>40779</v>
       </c>
       <c r="B37" s="9" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="C37" s="9" t="s">
         <v>13</v>
@@ -1495,7 +1432,7 @@
         <v>40796</v>
       </c>
       <c r="B38" s="10" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="C38" s="10" t="s">
         <v>5</v>
@@ -1519,7 +1456,7 @@
         <v>40813</v>
       </c>
       <c r="B39" s="9" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="C39" s="9" t="s">
         <v>13</v>
@@ -1543,7 +1480,7 @@
         <v>40830</v>
       </c>
       <c r="B40" s="9" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="C40" s="10" t="s">
         <v>9</v>
@@ -1567,7 +1504,7 @@
         <v>40847</v>
       </c>
       <c r="B41" s="10" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="C41" s="10" t="s">
         <v>18</v>
@@ -1591,7 +1528,7 @@
         <v>40864</v>
       </c>
       <c r="B42" s="9" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="C42" s="10" t="s">
         <v>6</v>
@@ -1615,7 +1552,7 @@
         <v>40881</v>
       </c>
       <c r="B43" s="9" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="C43" s="10" t="s">
         <v>6</v>
@@ -1639,7 +1576,7 @@
         <v>40898</v>
       </c>
       <c r="B44" s="10" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="C44" s="10" t="s">
         <v>18</v>
@@ -1666,135 +1603,4 @@
     <oddFooter>&amp;LDeveloped by Contextures Inc.&amp;Cwww.contextures.com&amp;R&amp;D</oddFooter>
   </headerFooter>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:B17"/>
-  <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="3" style="16" customWidth="1"/>
-    <col min="2" max="2" width="41.85546875" style="16" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="16"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1"/>
-      <c r="B1"/>
-    </row>
-    <row r="2" spans="1:2" ht="18" x14ac:dyDescent="0.25">
-      <c r="A2"/>
-      <c r="B2" s="18" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3"/>
-      <c r="B3"/>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4"/>
-      <c r="B4" s="17" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5"/>
-      <c r="B5" s="17" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6"/>
-      <c r="B6" s="17" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7"/>
-      <c r="B7" s="17" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8"/>
-      <c r="B8" s="17" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9"/>
-      <c r="B9"/>
-    </row>
-    <row r="10" spans="1:2" ht="18" x14ac:dyDescent="0.25">
-      <c r="A10"/>
-      <c r="B10" s="18" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11"/>
-      <c r="B11"/>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12"/>
-      <c r="B12" s="17" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13"/>
-      <c r="B13" s="17" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14"/>
-      <c r="B14" s="17" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15"/>
-      <c r="B15" s="17" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16"/>
-      <c r="B16" s="17" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B17" s="17" t="s">
-        <v>33</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B5" r:id="rId1"/>
-    <hyperlink ref="B7" r:id="rId2"/>
-    <hyperlink ref="B6" r:id="rId3"/>
-    <hyperlink ref="B12" r:id="rId4" tooltip="Jon Peltier's Excel Chart Utilities"/>
-    <hyperlink ref="B13" r:id="rId5" tooltip="ExcelUser Dashboards"/>
-    <hyperlink ref="B15" r:id="rId6" tooltip="Chandoo's Project Management Templates"/>
-    <hyperlink ref="B8" r:id="rId7" tooltip="Debra's Pivot Table Books on Amazon"/>
-    <hyperlink ref="B4" r:id="rId8" tooltip="30 Excel Functions in 30 Days eBook kit"/>
-    <hyperlink ref="B14" r:id="rId9" tooltip="Chandoo's Excel VBA School"/>
-    <hyperlink ref="B16" r:id="rId10" tooltip="Excel Guru Magic of Pivot Tables Course"/>
-    <hyperlink ref="B17" r:id="rId11" tooltip="JP's Random Data Generator for Excel"/>
-  </hyperlinks>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" r:id="rId12"/>
-  <headerFooter alignWithMargins="0">
-    <oddFooter>&amp;Lwww.contextures.com&amp;R&amp;D</oddFooter>
-  </headerFooter>
-</worksheet>
 </file>
</xml_diff>